<commit_message>
Retoques en las justificaciones
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Facultad\3 Año\DDS\TP-DDS-2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Ailén\UTN\DDS\TP-DDS-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927EAF6D-F31D-43E0-ACEE-5E2CA7026620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -140,48 +139,24 @@
     <t>Entrega 3</t>
   </si>
   <si>
-    <t>Categorizable</t>
-  </si>
-  <si>
     <t>La clase Item hereda de la clase categorizable.</t>
   </si>
   <si>
     <t>Creamos la clase "categorizable" para que todos los objetos que tengan que categorizarse utilize los atributos y métodos de esta clase, delegando la responsabilidad de de asignar categorias a los items.</t>
   </si>
   <si>
-    <t>Entidad</t>
-  </si>
-  <si>
     <t>Colocamos atributo criterios para llevar registro de los criterios adoptados por la organización</t>
   </si>
   <si>
-    <t>Ingreso</t>
-  </si>
-  <si>
-    <t>Egreso</t>
-  </si>
-  <si>
     <t>Relacionamos ambos colocando a cada uno como atributo del otro</t>
   </si>
   <si>
-    <t>Para asociar a ambos y que sea mas facil llevar registro de que ingreso perteneco a que egreso y viceversa</t>
-  </si>
-  <si>
     <t>Categoria</t>
   </si>
   <si>
     <t>La clase categoria conoce al criterio que pertenece</t>
   </si>
   <si>
-    <t>De esta forma cada Item (que hereda de Categorizable) tiene una lista de categorias y a su vez tambien conoce al criterio que pertenece.</t>
-  </si>
-  <si>
-    <t>El orden de la lista representa la jerarquia</t>
-  </si>
-  <si>
-    <t>Criterio</t>
-  </si>
-  <si>
     <t>El usuario ingresa los criterios en el orden de jerarquia</t>
   </si>
   <si>
@@ -189,13 +164,37 @@
   </si>
   <si>
     <t xml:space="preserve">De esta forma cada item conoce su jerarquia, porque conoce su criterio. </t>
+  </si>
+  <si>
+    <t>Item - Categorizable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidad </t>
+  </si>
+  <si>
+    <t>Entidad - Criterio</t>
+  </si>
+  <si>
+    <t>Egreso - Ingreso</t>
+  </si>
+  <si>
+    <t>Criterio - Categorizable</t>
+  </si>
+  <si>
+    <t>Para asociar a ambos y que sea mas facil llevar registro de en qué egreso se utilizó la plata de cierto ingreso.</t>
+  </si>
+  <si>
+    <t>De esta forma cada Item (que hereda de Categorizable) tiene una lista de categorias y a su vez tambien conoce el criterio al que pertenece cada una de sus categorías.</t>
+  </si>
+  <si>
+    <t>El orden de la lista representa la jerarquia (de primero al úlitmo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +207,14 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -217,7 +224,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -240,37 +247,29 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -365,23 +364,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -417,23 +399,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -609,11 +574,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,307 +607,307 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="5" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implementacion de scheduler y agrego clases de entrega 3
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Facultad\3 Año\DDS\TP-DDS-2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927EAF6D-F31D-43E0-ACEE-5E2CA7026620}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4997948-FE21-4775-9EC7-E3D7191D9D35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,9 +140,6 @@
     <t>Entrega 3</t>
   </si>
   <si>
-    <t>Categorizable</t>
-  </si>
-  <si>
     <t>La clase Item hereda de la clase categorizable.</t>
   </si>
   <si>
@@ -155,18 +152,9 @@
     <t>Colocamos atributo criterios para llevar registro de los criterios adoptados por la organización</t>
   </si>
   <si>
-    <t>Ingreso</t>
-  </si>
-  <si>
-    <t>Egreso</t>
-  </si>
-  <si>
     <t>Relacionamos ambos colocando a cada uno como atributo del otro</t>
   </si>
   <si>
-    <t>Para asociar a ambos y que sea mas facil llevar registro de que ingreso perteneco a que egreso y viceversa</t>
-  </si>
-  <si>
     <t>Categoria</t>
   </si>
   <si>
@@ -179,9 +167,6 @@
     <t>El orden de la lista representa la jerarquia</t>
   </si>
   <si>
-    <t>Criterio</t>
-  </si>
-  <si>
     <t>El usuario ingresa los criterios en el orden de jerarquia</t>
   </si>
   <si>
@@ -189,6 +174,21 @@
   </si>
   <si>
     <t xml:space="preserve">De esta forma cada item conoce su jerarquia, porque conoce su criterio. </t>
+  </si>
+  <si>
+    <t>Item,Categorizable</t>
+  </si>
+  <si>
+    <t>Egreso,Ingreso</t>
+  </si>
+  <si>
+    <t>Criterio, Entidad</t>
+  </si>
+  <si>
+    <t>Criterio, Categorizable</t>
+  </si>
+  <si>
+    <t>Para asociar a ambos y que sea mas facil llevar registro de que ingreso pertenece a que egreso y viceversa</t>
   </si>
 </sst>
 </file>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,90 +816,90 @@
     </row>
     <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cambio justificaciones y diagrama
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Facultad\3 Año\DDS\TP-DDS-2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eze\Desktop\UTN\Diseño de Sistemas\TP DDS (consola)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4997948-FE21-4775-9EC7-E3D7191D9D35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDDCEC6-1280-40E8-87CB-C804BC605C55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>Decisión</t>
   </si>
@@ -189,13 +189,34 @@
   </si>
   <si>
     <t>Para asociar a ambos y que sea mas facil llevar registro de que ingreso pertenece a que egreso y viceversa</t>
+  </si>
+  <si>
+    <t>Entrega 4</t>
+  </si>
+  <si>
+    <t>Vinculador</t>
+  </si>
+  <si>
+    <t>Encapsulamos el proceso del validador en una clase que se encarga de recibir la entidad y los criterios con los que quiere vincular</t>
+  </si>
+  <si>
+    <t>Hacer un Strategy y una clase para cada metodo de validacion</t>
+  </si>
+  <si>
+    <t>Item, ItemEgreso, ItemPresupuesto</t>
+  </si>
+  <si>
+    <t>Sacamos la clase Item y Separamos al item del egreso del item del ingreso para tratarlos como objetos diferentes</t>
+  </si>
+  <si>
+    <t>Hacer que ItemEgreso e ItemPresupuesto hereden de la misma clase item, no pudimos hacerlo asi por limitaciones del ORM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +228,14 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -255,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -270,6 +299,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -612,19 +644,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="1" max="2" width="24.83984375" customWidth="1"/>
+    <col min="3" max="3" width="25.15625" customWidth="1"/>
+    <col min="4" max="4" width="22.578125" customWidth="1"/>
+    <col min="5" max="5" width="31.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -641,7 +673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -656,7 +688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -671,7 +703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -686,7 +718,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -701,7 +733,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -716,7 +748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -731,7 +763,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -746,7 +778,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -761,7 +793,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
@@ -776,7 +808,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -791,14 +823,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -807,14 +839,14 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -829,7 +861,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -842,7 +874,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -857,7 +889,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
@@ -872,7 +904,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -887,7 +919,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -902,42 +934,60 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>

</xml_diff>

<commit_message>
modificacion de decisiones de diseño
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eze\Desktop\UTN\Diseño de Sistemas\TP DDS (consola)\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDDCEC6-1280-40E8-87CB-C804BC605C55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>Decisión</t>
   </si>
@@ -65,12 +59,6 @@
     <t>Tenemos al egreso y a los presupuestos relacionados por una misma compra. El egreso y la lista de presupuestos son atributos de la compra.</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Tenemos solamente una clase Item y una calse Producto.</t>
-  </si>
-  <si>
     <t>Compra, Presupuesto</t>
   </si>
   <si>
@@ -128,24 +116,9 @@
     <t>Documento Comercial, Presupuesto</t>
   </si>
   <si>
-    <t>Hicimos dos tablas, una para cada uno.</t>
-  </si>
-  <si>
-    <t>Porque en el caso que un documento comercial no sea un presupuesto, son muchos campos que quedarian vacios.</t>
-  </si>
-  <si>
-    <t>Hasta ahora no nos parecio necesario incorporar una clase que identifique al Producto ya que solo estamos modelando compras de la empresa a provedores.</t>
-  </si>
-  <si>
     <t>Entrega 3</t>
   </si>
   <si>
-    <t>La clase Item hereda de la clase categorizable.</t>
-  </si>
-  <si>
-    <t>Creamos la clase "categorizable" para que todos los objetos que tengan que categorizarse utilize los atributos y métodos de esta clase, delegando la responsabilidad de de asignar categorias a los items.</t>
-  </si>
-  <si>
     <t>Entidad</t>
   </si>
   <si>
@@ -176,9 +149,6 @@
     <t xml:space="preserve">De esta forma cada item conoce su jerarquia, porque conoce su criterio. </t>
   </si>
   <si>
-    <t>Item,Categorizable</t>
-  </si>
-  <si>
     <t>Egreso,Ingreso</t>
   </si>
   <si>
@@ -210,12 +180,48 @@
   </si>
   <si>
     <t>Hacer que ItemEgreso e ItemPresupuesto hereden de la misma clase item, no pudimos hacerlo asi por limitaciones del ORM</t>
+  </si>
+  <si>
+    <t>Hicimos una sola tabla para las dos clases.</t>
+  </si>
+  <si>
+    <t>El tipo de herencia que implementamos es un TPH, porque resulta más fácil la implementación con el ORM.</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Entidad, EntidadJuridica, EntidadBase</t>
+  </si>
+  <si>
+    <t>Se decidió utilizar la herencia TPH para hacer las tablas</t>
+  </si>
+  <si>
+    <t>Se decidió utilizar la herencia TPT para hacer las tablas</t>
+  </si>
+  <si>
+    <t>La razón es porque se necesita que las entidades se encuentren separadas para poder hacer luego la composición de la EntidadBase y la EntidadJurídica.</t>
+  </si>
+  <si>
+    <t>TipoEmpresa, Micro, Pequenia, MedianaTramo1, MedianaTramo2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El tipo de herencia que implementamos es un TPH, porque resulta más fácil la implementación </t>
+  </si>
+  <si>
+    <t>Componente</t>
+  </si>
+  <si>
+    <t>Se decidió no incluir a Brasil</t>
+  </si>
+  <si>
+    <t>Tiene demasiadas ciudades y ralentiza demasiado el programa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -322,7 +328,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -364,7 +370,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,26 +403,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,23 +438,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -641,22 +613,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.83984375" customWidth="1"/>
-    <col min="3" max="3" width="25.15625" customWidth="1"/>
-    <col min="4" max="4" width="22.578125" customWidth="1"/>
-    <col min="5" max="5" width="31.83984375" customWidth="1"/>
+    <col min="1" max="2" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="31.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -715,37 +687,29 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -753,29 +717,29 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -783,44 +747,44 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -832,7 +796,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -846,153 +810,190 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>39</v>
-      </c>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="67.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="5" t="s">
-        <v>56</v>
-      </c>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>59</v>
-      </c>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="5"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+    <row r="25" spans="1:5" ht="83.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+    <row r="26" spans="1:5" ht="85.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agrego decisiones de diseño
</commit_message>
<xml_diff>
--- a/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
+++ b/Justificaciones-de-Decisiones-para-TP-Anual.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eze\Desktop\UTN\Diseño de Sistemas\TP DDS (consola)\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37713178-183D-4D49-A2CE-6F0DE93F7101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552"/>
+    <workbookView xWindow="12768" yWindow="1776" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -164,24 +170,9 @@
     <t>Entrega 4</t>
   </si>
   <si>
-    <t>Vinculador</t>
-  </si>
-  <si>
-    <t>Encapsulamos el proceso del validador en una clase que se encarga de recibir la entidad y los criterios con los que quiere vincular</t>
-  </si>
-  <si>
-    <t>Hacer un Strategy y una clase para cada metodo de validacion</t>
-  </si>
-  <si>
     <t>Item, ItemEgreso, ItemPresupuesto</t>
   </si>
   <si>
-    <t>Sacamos la clase Item y Separamos al item del egreso del item del ingreso para tratarlos como objetos diferentes</t>
-  </si>
-  <si>
-    <t>Hacer que ItemEgreso e ItemPresupuesto hereden de la misma clase item, no pudimos hacerlo asi por limitaciones del ORM</t>
-  </si>
-  <si>
     <t>Hicimos una sola tabla para las dos clases.</t>
   </si>
   <si>
@@ -209,20 +200,35 @@
     <t xml:space="preserve">El tipo de herencia que implementamos es un TPH, porque resulta más fácil la implementación </t>
   </si>
   <si>
-    <t>Componente</t>
-  </si>
-  <si>
-    <t>Se decidió no incluir a Brasil</t>
-  </si>
-  <si>
-    <t>Tiene demasiadas ciudades y ralentiza demasiado el programa</t>
+    <t xml:space="preserve">Agregamos dos clases que heredan de Item, ItemEgreso e ItemPresupuesto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porque nos parecio mejor tratarlos polimorficamente pero como objetos diferentes. Ademas se nos hacia dificil persistir una unica clase item que se pueda relacionar con dos entidades diferentes </t>
+  </si>
+  <si>
+    <t>En la persistencia de paises solo incluimos a Argentina</t>
+  </si>
+  <si>
+    <t>Porque sino es un volumen muy grande de datos que no sabemos si son necesarios y relentiza la carga de informacion a la BD</t>
+  </si>
+  <si>
+    <t>Base de datos</t>
+  </si>
+  <si>
+    <t>Vinculador Ingresos-Egresos</t>
+  </si>
+  <si>
+    <t>Encapsulamos el proceso del vinculador en una clase que se encarga de recibir la entidad y los criterios con los que quiere vincular</t>
+  </si>
+  <si>
+    <t>Hacer un Strategy y una clase para cada metodo de vinculador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,14 +240,6 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -290,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -305,10 +303,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -328,7 +329,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -370,7 +371,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -403,9 +404,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,6 +456,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -613,22 +648,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5234375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" customWidth="1"/>
+    <col min="1" max="2" width="24.89453125" customWidth="1"/>
+    <col min="3" max="3" width="25.1015625" customWidth="1"/>
+    <col min="4" max="4" width="22.5234375" customWidth="1"/>
+    <col min="5" max="5" width="31.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="36.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -660,7 +695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -690,7 +725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
@@ -727,7 +762,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -757,7 +792,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -772,7 +807,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -780,11 +815,11 @@
         <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -810,14 +845,14 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -875,7 +910,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5" t="s">
         <v>5</v>
       </c>
@@ -890,21 +925,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -922,16 +957,16 @@
     </row>
     <row r="25" spans="1:5" ht="83.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E25" s="5"/>
     </row>
@@ -940,60 +975,193 @@
         <v>5</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="C27" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="49.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="C28" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="C29" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
-        <v>66</v>
-      </c>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="5"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>